<commit_message>
trying to limit using CPU and memory to 80%
</commit_message>
<xml_diff>
--- a/Datasets_metadata.xlsx
+++ b/Datasets_metadata.xlsx
@@ -810,6 +810,139 @@
   </cellStyles>
   <dxfs count="32">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1071,6 +1204,227 @@
       </fill>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1089,360 +1443,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1464,18 +1464,18 @@
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="dataset" dataDxfId="9"/>
-    <tableColumn id="7" name="uea_ucr" dataDxfId="8"/>
-    <tableColumn id="8" name="in_both" dataDxfId="7">
+    <tableColumn id="1" name="dataset" dataDxfId="29"/>
+    <tableColumn id="7" name="uea_ucr" dataDxfId="28"/>
+    <tableColumn id="8" name="in_both" dataDxfId="27">
       <calculatedColumnFormula>IF(Table1[[#This Row],[dataset]]=Table1[[#This Row],[uea_ucr]],TRUE,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="train_size" dataDxfId="6"/>
-    <tableColumn id="3" name="test_size" dataDxfId="5"/>
-    <tableColumn id="4" name="length" dataDxfId="4"/>
-    <tableColumn id="5" name="num_classes" dataDxfId="3"/>
-    <tableColumn id="6" name="type" dataDxfId="2"/>
-    <tableColumn id="11" name="dim" dataDxfId="1"/>
-    <tableColumn id="10" name="num_dim" dataDxfId="0"/>
+    <tableColumn id="2" name="train_size" dataDxfId="26"/>
+    <tableColumn id="3" name="test_size" dataDxfId="25"/>
+    <tableColumn id="4" name="length" dataDxfId="24"/>
+    <tableColumn id="5" name="num_classes" dataDxfId="23"/>
+    <tableColumn id="6" name="type" dataDxfId="22"/>
+    <tableColumn id="11" name="dim" dataDxfId="21"/>
+    <tableColumn id="10" name="num_dim" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1494,24 +1494,24 @@
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="dataset" dataDxfId="31"/>
-    <tableColumn id="7" name="uea_ucr" dataDxfId="30"/>
-    <tableColumn id="8" name="in_both" dataDxfId="29">
+    <tableColumn id="1" name="dataset" dataDxfId="15"/>
+    <tableColumn id="7" name="uea_ucr" dataDxfId="14"/>
+    <tableColumn id="8" name="in_both" dataDxfId="13">
       <calculatedColumnFormula>IF(Table13[[#This Row],[dataset]]=Table13[[#This Row],[uea_ucr]],TRUE,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="type" dataDxfId="28"/>
-    <tableColumn id="11" name="dim" dataDxfId="27"/>
-    <tableColumn id="9" name="knn_ed" dataDxfId="26"/>
-    <tableColumn id="10" name="knn_dtw" dataDxfId="25"/>
-    <tableColumn id="12" name="knn_msm" dataDxfId="24"/>
-    <tableColumn id="13" name="pforest" dataDxfId="23"/>
-    <tableColumn id="14" name="ls" dataDxfId="22"/>
-    <tableColumn id="15" name="st" dataDxfId="21"/>
-    <tableColumn id="16" name="tsf" dataDxfId="20"/>
-    <tableColumn id="17" name="weasel" dataDxfId="19"/>
-    <tableColumn id="18" name="boss" dataDxfId="18"/>
-    <tableColumn id="19" name="inception" dataDxfId="17"/>
-    <tableColumn id="20" name="finished_algo" dataDxfId="16">
+    <tableColumn id="6" name="type" dataDxfId="12"/>
+    <tableColumn id="11" name="dim" dataDxfId="11"/>
+    <tableColumn id="9" name="knn_ed" dataDxfId="10"/>
+    <tableColumn id="10" name="knn_dtw" dataDxfId="9"/>
+    <tableColumn id="12" name="knn_msm" dataDxfId="8"/>
+    <tableColumn id="13" name="pforest" dataDxfId="7"/>
+    <tableColumn id="14" name="ls" dataDxfId="6"/>
+    <tableColumn id="15" name="st" dataDxfId="5"/>
+    <tableColumn id="16" name="tsf" dataDxfId="4"/>
+    <tableColumn id="17" name="weasel" dataDxfId="3"/>
+    <tableColumn id="18" name="boss" dataDxfId="2"/>
+    <tableColumn id="19" name="inception" dataDxfId="1"/>
+    <tableColumn id="20" name="finished_algo" dataDxfId="0">
       <calculatedColumnFormula>SUM(F2:O2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1785,7 +1785,7 @@
   <dimension ref="A1:J179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="J121" sqref="A121:J121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7587,10 +7587,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C179">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13323,18 +13323,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C93 C101:C180">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:C100">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixed splitting from the back, fixed distance measures for pforest, fixed indexes for splitted data
</commit_message>
<xml_diff>
--- a/Datasets_metadata.xlsx
+++ b/Datasets_metadata.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="224">
   <si>
     <t>AbnormalHeartbeat</t>
   </si>
@@ -694,6 +695,9 @@
   </si>
   <si>
     <t>num_dim</t>
+  </si>
+  <si>
+    <t>balanced</t>
   </si>
 </sst>
 </file>
@@ -789,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -804,11 +808,74 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1164,46 +1231,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1424,26 +1451,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1459,23 +1466,48 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J179" totalsRowShown="0">
-  <autoFilter ref="A1:J179"/>
-  <sortState ref="A2:H179">
-    <sortCondition ref="A1:A179"/>
+  <autoFilter ref="A1:J179">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="AUDIO"/>
+        <filter val="DEVICE"/>
+        <filter val="ECG"/>
+        <filter val="EEG"/>
+        <filter val="EOG"/>
+        <filter val="EPG"/>
+        <filter val="HAR"/>
+        <filter val="HEMODYNAMICS"/>
+        <filter val="MISC"/>
+        <filter val="OTHER"/>
+        <filter val="SENSOR"/>
+        <filter val="SOUND"/>
+        <filter val="SPECTRO"/>
+        <filter val="SPEECH"/>
+        <filter val="Traffic"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A3:J175">
+    <sortCondition ref="B1:B179"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="dataset" dataDxfId="29"/>
-    <tableColumn id="7" name="uea_ucr" dataDxfId="28"/>
-    <tableColumn id="8" name="in_both" dataDxfId="27">
+    <tableColumn id="1" name="dataset" dataDxfId="31"/>
+    <tableColumn id="7" name="uea_ucr" dataDxfId="30"/>
+    <tableColumn id="8" name="in_both" dataDxfId="29">
       <calculatedColumnFormula>IF(Table1[[#This Row],[dataset]]=Table1[[#This Row],[uea_ucr]],TRUE,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="train_size" dataDxfId="26"/>
-    <tableColumn id="3" name="test_size" dataDxfId="25"/>
-    <tableColumn id="4" name="length" dataDxfId="24"/>
-    <tableColumn id="5" name="num_classes" dataDxfId="23"/>
-    <tableColumn id="6" name="type" dataDxfId="22"/>
-    <tableColumn id="11" name="dim" dataDxfId="21"/>
-    <tableColumn id="10" name="num_dim" dataDxfId="20"/>
+    <tableColumn id="2" name="train_size" dataDxfId="28"/>
+    <tableColumn id="3" name="test_size" dataDxfId="27"/>
+    <tableColumn id="4" name="length" dataDxfId="26"/>
+    <tableColumn id="5" name="num_classes" dataDxfId="25"/>
+    <tableColumn id="6" name="type" dataDxfId="24"/>
+    <tableColumn id="11" name="dim" dataDxfId="23"/>
+    <tableColumn id="10" name="num_dim" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1494,26 +1526,49 @@
     <sortCondition ref="A1:A179"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" name="dataset" dataDxfId="15"/>
-    <tableColumn id="7" name="uea_ucr" dataDxfId="14"/>
-    <tableColumn id="8" name="in_both" dataDxfId="13">
+    <tableColumn id="1" name="dataset" dataDxfId="21"/>
+    <tableColumn id="7" name="uea_ucr" dataDxfId="20"/>
+    <tableColumn id="8" name="in_both" dataDxfId="19">
       <calculatedColumnFormula>IF(Table13[[#This Row],[dataset]]=Table13[[#This Row],[uea_ucr]],TRUE,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="type" dataDxfId="12"/>
-    <tableColumn id="11" name="dim" dataDxfId="11"/>
-    <tableColumn id="9" name="knn_ed" dataDxfId="10"/>
-    <tableColumn id="10" name="knn_dtw" dataDxfId="9"/>
-    <tableColumn id="12" name="knn_msm" dataDxfId="8"/>
-    <tableColumn id="13" name="pforest" dataDxfId="7"/>
-    <tableColumn id="14" name="ls" dataDxfId="6"/>
-    <tableColumn id="15" name="st" dataDxfId="5"/>
-    <tableColumn id="16" name="tsf" dataDxfId="4"/>
-    <tableColumn id="17" name="weasel" dataDxfId="3"/>
-    <tableColumn id="18" name="boss" dataDxfId="2"/>
-    <tableColumn id="19" name="inception" dataDxfId="1"/>
-    <tableColumn id="20" name="finished_algo" dataDxfId="0">
+    <tableColumn id="6" name="type" dataDxfId="18"/>
+    <tableColumn id="11" name="dim" dataDxfId="17"/>
+    <tableColumn id="9" name="knn_ed" dataDxfId="16"/>
+    <tableColumn id="10" name="knn_dtw" dataDxfId="15"/>
+    <tableColumn id="12" name="knn_msm" dataDxfId="14"/>
+    <tableColumn id="13" name="pforest" dataDxfId="13"/>
+    <tableColumn id="14" name="ls" dataDxfId="12"/>
+    <tableColumn id="15" name="st" dataDxfId="11"/>
+    <tableColumn id="16" name="tsf" dataDxfId="10"/>
+    <tableColumn id="17" name="weasel" dataDxfId="9"/>
+    <tableColumn id="18" name="boss" dataDxfId="8"/>
+    <tableColumn id="19" name="inception" dataDxfId="7"/>
+    <tableColumn id="20" name="finished_algo" dataDxfId="6">
       <calculatedColumnFormula>SUM(F2:O2)</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K88" totalsRowShown="0">
+  <autoFilter ref="A1:K88"/>
+  <sortState ref="A2:K88">
+    <sortCondition ref="A1:A88"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" name="dataset"/>
+    <tableColumn id="2" name="uea_ucr"/>
+    <tableColumn id="3" name="in_both"/>
+    <tableColumn id="4" name="train_size"/>
+    <tableColumn id="5" name="test_size"/>
+    <tableColumn id="6" name="length"/>
+    <tableColumn id="7" name="num_classes"/>
+    <tableColumn id="8" name="type"/>
+    <tableColumn id="9" name="dim"/>
+    <tableColumn id="10" name="num_dim"/>
+    <tableColumn id="11" name="balanced"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1782,10 +1837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J179"/>
+  <dimension ref="A1:N179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J121" sqref="A121:J121"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1799,6 +1854,7 @@
     <col min="8" max="8" width="15.21875" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1833,7 +1889,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1893,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1926,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1959,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1992,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2025,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -2058,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -2091,7 +2147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -2118,7 +2174,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -2145,7 +2201,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2172,7 +2228,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2199,7 +2255,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -2226,7 +2282,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
@@ -2352,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
@@ -2385,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
@@ -2412,7 +2468,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
@@ -2445,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>27</v>
       </c>
@@ -2511,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
@@ -2538,7 +2594,7 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
@@ -2571,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
@@ -2637,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
@@ -2736,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -2796,7 +2852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>41</v>
       </c>
@@ -2823,7 +2879,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
@@ -2855,8 +2911,9 @@
       <c r="J34" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N34" s="10"/>
+    </row>
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
@@ -2888,8 +2945,9 @@
       <c r="J35" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N35" s="10"/>
+    </row>
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
@@ -2921,8 +2979,9 @@
       <c r="J36" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N36" s="10"/>
+    </row>
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>45</v>
       </c>
@@ -2954,8 +3013,9 @@
       <c r="J37" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N37" s="10"/>
+    </row>
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>46</v>
       </c>
@@ -2987,8 +3047,9 @@
       <c r="J38" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N38" s="10"/>
+    </row>
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>47</v>
       </c>
@@ -3020,8 +3081,9 @@
       <c r="J39" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N39" s="10"/>
+    </row>
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>48</v>
       </c>
@@ -3053,8 +3115,9 @@
       <c r="J40" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N40" s="10"/>
+    </row>
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>49</v>
       </c>
@@ -3086,8 +3149,9 @@
       <c r="J41" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N41" s="10"/>
+    </row>
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>50</v>
       </c>
@@ -3119,8 +3183,9 @@
       <c r="J42" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N42" s="10"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>51</v>
       </c>
@@ -3152,8 +3217,9 @@
       <c r="J43" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N43" s="10"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>52</v>
       </c>
@@ -3185,8 +3251,9 @@
       <c r="J44" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N44" s="10"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>53</v>
       </c>
@@ -3218,8 +3285,9 @@
       <c r="J45" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N45" s="10"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>54</v>
       </c>
@@ -3251,8 +3319,9 @@
       <c r="J46" s="4">
         <v>1345</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="N46" s="10"/>
+    </row>
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>55</v>
       </c>
@@ -3279,7 +3348,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>56</v>
       </c>
@@ -3411,7 +3480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>60</v>
       </c>
@@ -3444,7 +3513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>61</v>
       </c>
@@ -3700,7 +3769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>71</v>
       </c>
@@ -3727,7 +3796,7 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>73</v>
       </c>
@@ -3793,7 +3862,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>75</v>
       </c>
@@ -3826,7 +3895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>76</v>
       </c>
@@ -3859,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>77</v>
       </c>
@@ -3925,7 +3994,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>79</v>
       </c>
@@ -4090,7 +4159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>84</v>
       </c>
@@ -4150,7 +4219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>86</v>
       </c>
@@ -4183,7 +4252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>87</v>
       </c>
@@ -4216,7 +4285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>88</v>
       </c>
@@ -4249,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>89</v>
       </c>
@@ -4282,7 +4351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>90</v>
       </c>
@@ -4315,7 +4384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>91</v>
       </c>
@@ -4348,7 +4417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>92</v>
       </c>
@@ -4381,7 +4450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>93</v>
       </c>
@@ -4414,7 +4483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>94</v>
       </c>
@@ -4513,7 +4582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>97</v>
       </c>
@@ -4579,7 +4648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>99</v>
       </c>
@@ -4645,7 +4714,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>101</v>
       </c>
@@ -4711,7 +4780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>103</v>
       </c>
@@ -4812,23 +4881,23 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>199</v>
+        <v>108</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C95" s="7" t="b">
+        <v>108</v>
+      </c>
+      <c r="C95" s="5" t="b">
         <f>IF(Table1[[#This Row],[dataset]]=Table1[[#This Row],[uea_ucr]],TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D95" s="5">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="E95" s="5">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="F95" s="5">
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="G95" s="5">
         <v>10</v>
@@ -4837,31 +4906,31 @@
         <v>1</v>
       </c>
       <c r="I95" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J95" s="4">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>108</v>
+        <v>199</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C96" s="5" t="b">
+        <v>199</v>
+      </c>
+      <c r="C96" s="7" t="b">
         <f>IF(Table1[[#This Row],[dataset]]=Table1[[#This Row],[uea_ucr]],TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="D96" s="5">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="E96" s="5">
-        <v>20000</v>
+        <v>25000</v>
       </c>
       <c r="F96" s="5">
-        <v>30</v>
+        <v>600</v>
       </c>
       <c r="G96" s="5">
         <v>10</v>
@@ -4870,10 +4939,10 @@
         <v>1</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J96" s="4">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
@@ -5107,7 +5176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>116</v>
       </c>
@@ -5173,7 +5242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>118</v>
       </c>
@@ -5239,7 +5308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>121</v>
       </c>
@@ -5272,7 +5341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>122</v>
       </c>
@@ -5305,7 +5374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>123</v>
       </c>
@@ -5338,7 +5407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>124</v>
       </c>
@@ -5371,7 +5440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>125</v>
       </c>
@@ -5404,7 +5473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>126</v>
       </c>
@@ -5629,7 +5698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>133</v>
       </c>
@@ -5695,7 +5764,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>136</v>
       </c>
@@ -5728,7 +5797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>137</v>
       </c>
@@ -5794,7 +5863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>140</v>
       </c>
@@ -6058,7 +6127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>149</v>
       </c>
@@ -6091,7 +6160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>150</v>
       </c>
@@ -6124,7 +6193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>151</v>
       </c>
@@ -6223,7 +6292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>154</v>
       </c>
@@ -6514,7 +6583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
         <v>163</v>
       </c>
@@ -6547,7 +6616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
         <v>164</v>
       </c>
@@ -6580,7 +6649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
         <v>165</v>
       </c>
@@ -6640,7 +6709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
         <v>168</v>
       </c>
@@ -6871,7 +6940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="4" t="s">
         <v>176</v>
       </c>
@@ -6904,7 +6973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
         <v>177</v>
       </c>
@@ -6937,7 +7006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
         <v>178</v>
       </c>
@@ -6970,7 +7039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
         <v>179</v>
       </c>
@@ -6997,7 +7066,7 @@
       <c r="I161" s="4"/>
       <c r="J161" s="4"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="4" t="s">
         <v>180</v>
       </c>
@@ -7030,7 +7099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>181</v>
       </c>
@@ -7129,7 +7198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
         <v>184</v>
       </c>
@@ -7162,7 +7231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>185</v>
       </c>
@@ -7195,7 +7264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>186</v>
       </c>
@@ -7255,7 +7324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
         <v>188</v>
       </c>
@@ -7288,7 +7357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
         <v>189</v>
       </c>
@@ -7321,7 +7390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
         <v>190</v>
       </c>
@@ -7354,7 +7423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="4" t="s">
         <v>191</v>
       </c>
@@ -7453,7 +7522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
         <v>194</v>
       </c>
@@ -7486,7 +7555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
         <v>195</v>
       </c>
@@ -7519,7 +7588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="4" t="s">
         <v>196</v>
       </c>
@@ -7552,7 +7621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="4" t="s">
         <v>197</v>
       </c>
@@ -7587,10 +7656,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C179">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13323,18 +13392,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C93 C101:C180">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:C100">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13343,4 +13412,3116 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>1460</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>640</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>470</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <v>577</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>200</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>345</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>200</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>1380</v>
+      </c>
+      <c r="F8">
+        <v>1639</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>200</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>286</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>200</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="12"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>250</v>
+      </c>
+      <c r="E10">
+        <v>250</v>
+      </c>
+      <c r="F10">
+        <v>720</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>200</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>108</v>
+      </c>
+      <c r="E11">
+        <v>72</v>
+      </c>
+      <c r="F11">
+        <v>1197</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>80</v>
+      </c>
+      <c r="F12">
+        <v>288</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
+        <v>200</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>138</v>
+      </c>
+      <c r="F13">
+        <v>288</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" t="s">
+        <v>200</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>138</v>
+      </c>
+      <c r="F14">
+        <v>288</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" t="s">
+        <v>200</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>60</v>
+      </c>
+      <c r="E15">
+        <v>40</v>
+      </c>
+      <c r="F15">
+        <v>270</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>201</v>
+      </c>
+      <c r="J15">
+        <v>1345</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>322</v>
+      </c>
+      <c r="E16">
+        <v>139</v>
+      </c>
+      <c r="F16">
+        <v>512</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" t="s">
+        <v>200</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>96</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
+        <v>200</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>500</v>
+      </c>
+      <c r="E18">
+        <v>4500</v>
+      </c>
+      <c r="F18">
+        <v>140</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>200</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <v>861</v>
+      </c>
+      <c r="F19">
+        <v>136</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>200</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>8926</v>
+      </c>
+      <c r="E20">
+        <v>7711</v>
+      </c>
+      <c r="F20">
+        <v>96</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>200</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>362</v>
+      </c>
+      <c r="E21">
+        <v>362</v>
+      </c>
+      <c r="F21">
+        <v>1250</v>
+      </c>
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" t="s">
+        <v>200</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>362</v>
+      </c>
+      <c r="E22">
+        <v>362</v>
+      </c>
+      <c r="F22">
+        <v>1250</v>
+      </c>
+      <c r="G22">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" t="s">
+        <v>200</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>137</v>
+      </c>
+      <c r="E23">
+        <v>138</v>
+      </c>
+      <c r="F23">
+        <v>207</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>201</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>30</v>
+      </c>
+      <c r="E24">
+        <v>270</v>
+      </c>
+      <c r="F24">
+        <v>65</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>201</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>261</v>
+      </c>
+      <c r="E25">
+        <v>263</v>
+      </c>
+      <c r="F25">
+        <v>1751</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>504</v>
+      </c>
+      <c r="E26">
+        <v>500</v>
+      </c>
+      <c r="F26">
+        <v>1751</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" t="s">
+        <v>200</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>5890</v>
+      </c>
+      <c r="E27">
+        <v>3524</v>
+      </c>
+      <c r="F27">
+        <v>62</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" t="s">
+        <v>201</v>
+      </c>
+      <c r="J27">
+        <v>144</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>316</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" t="s">
+        <v>201</v>
+      </c>
+      <c r="J28">
+        <v>28</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>3601</v>
+      </c>
+      <c r="E29">
+        <v>1320</v>
+      </c>
+      <c r="F29">
+        <v>500</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" t="s">
+        <v>200</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>3636</v>
+      </c>
+      <c r="E30">
+        <v>810</v>
+      </c>
+      <c r="F30">
+        <v>500</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" t="s">
+        <v>200</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>150</v>
+      </c>
+      <c r="E31">
+        <v>2850</v>
+      </c>
+      <c r="F31">
+        <v>301</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" t="s">
+        <v>200</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>28</v>
+      </c>
+      <c r="E32">
+        <v>2850</v>
+      </c>
+      <c r="F32">
+        <v>301</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" t="s">
+        <v>200</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>18</v>
+      </c>
+      <c r="E33">
+        <v>186</v>
+      </c>
+      <c r="F33">
+        <v>201</v>
+      </c>
+      <c r="G33">
+        <v>18</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33" t="s">
+        <v>200</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>109</v>
+      </c>
+      <c r="E34">
+        <v>105</v>
+      </c>
+      <c r="F34">
+        <v>431</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" t="s">
+        <v>200</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>160</v>
+      </c>
+      <c r="E35">
+        <v>74</v>
+      </c>
+      <c r="F35">
+        <v>400</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I35" t="s">
+        <v>201</v>
+      </c>
+      <c r="J35">
+        <v>10</v>
+      </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>150</v>
+      </c>
+      <c r="E36">
+        <v>850</v>
+      </c>
+      <c r="F36">
+        <v>152</v>
+      </c>
+      <c r="G36">
+        <v>26</v>
+      </c>
+      <c r="H36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" t="s">
+        <v>201</v>
+      </c>
+      <c r="J36">
+        <v>3</v>
+      </c>
+      <c r="K36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>204</v>
+      </c>
+      <c r="E37">
+        <v>205</v>
+      </c>
+      <c r="F37">
+        <v>405</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>201</v>
+      </c>
+      <c r="J37">
+        <v>61</v>
+      </c>
+      <c r="K37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>34</v>
+      </c>
+      <c r="E38">
+        <v>101</v>
+      </c>
+      <c r="F38">
+        <v>3000</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>3</v>
+      </c>
+      <c r="I38" t="s">
+        <v>200</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>62</v>
+      </c>
+      <c r="E39">
+        <v>249</v>
+      </c>
+      <c r="F39">
+        <v>601</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39" t="s">
+        <v>105</v>
+      </c>
+      <c r="I39" t="s">
+        <v>200</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>17</v>
+      </c>
+      <c r="E40">
+        <v>249</v>
+      </c>
+      <c r="F40">
+        <v>601</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40" t="s">
+        <v>105</v>
+      </c>
+      <c r="I40" t="s">
+        <v>200</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>30000</v>
+      </c>
+      <c r="E41">
+        <v>20000</v>
+      </c>
+      <c r="F41">
+        <v>30</v>
+      </c>
+      <c r="G41">
+        <v>10</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>201</v>
+      </c>
+      <c r="J41">
+        <v>200</v>
+      </c>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42" t="s">
+        <v>199</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>25000</v>
+      </c>
+      <c r="E42">
+        <v>25000</v>
+      </c>
+      <c r="F42">
+        <v>600</v>
+      </c>
+      <c r="G42">
+        <v>10</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>200</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>67</v>
+      </c>
+      <c r="E43">
+        <v>1029</v>
+      </c>
+      <c r="F43">
+        <v>24</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" t="s">
+        <v>200</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>270</v>
+      </c>
+      <c r="E44">
+        <v>370</v>
+      </c>
+      <c r="F44">
+        <v>29</v>
+      </c>
+      <c r="G44">
+        <v>9</v>
+      </c>
+      <c r="H44" t="s">
+        <v>1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>201</v>
+      </c>
+      <c r="J44">
+        <v>12</v>
+      </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>375</v>
+      </c>
+      <c r="E45">
+        <v>375</v>
+      </c>
+      <c r="F45">
+        <v>720</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45" t="s">
+        <v>3</v>
+      </c>
+      <c r="I45" t="s">
+        <v>200</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>180</v>
+      </c>
+      <c r="E46">
+        <v>180</v>
+      </c>
+      <c r="F46">
+        <v>45</v>
+      </c>
+      <c r="G46">
+        <v>15</v>
+      </c>
+      <c r="H46" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" t="s">
+        <v>201</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>60</v>
+      </c>
+      <c r="E47">
+        <v>61</v>
+      </c>
+      <c r="F47">
+        <v>637</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47" t="s">
+        <v>30</v>
+      </c>
+      <c r="I47" t="s">
+        <v>200</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>70</v>
+      </c>
+      <c r="E48">
+        <v>73</v>
+      </c>
+      <c r="F48">
+        <v>319</v>
+      </c>
+      <c r="G48">
+        <v>7</v>
+      </c>
+      <c r="H48" t="s">
+        <v>30</v>
+      </c>
+      <c r="I48" t="s">
+        <v>200</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>2459</v>
+      </c>
+      <c r="E49">
+        <v>2466</v>
+      </c>
+      <c r="F49">
+        <v>36</v>
+      </c>
+      <c r="G49">
+        <v>14</v>
+      </c>
+      <c r="H49" t="s">
+        <v>69</v>
+      </c>
+      <c r="I49" t="s">
+        <v>201</v>
+      </c>
+      <c r="J49">
+        <v>6</v>
+      </c>
+      <c r="K49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>60</v>
+      </c>
+      <c r="E50">
+        <v>60</v>
+      </c>
+      <c r="F50">
+        <v>448</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50" t="s">
+        <v>23</v>
+      </c>
+      <c r="I50" t="s">
+        <v>200</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1194</v>
+      </c>
+      <c r="E51">
+        <v>2439</v>
+      </c>
+      <c r="F51">
+        <v>24</v>
+      </c>
+      <c r="G51">
+        <v>10</v>
+      </c>
+      <c r="H51" t="s">
+        <v>120</v>
+      </c>
+      <c r="I51" t="s">
+        <v>200</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>20</v>
+      </c>
+      <c r="E52">
+        <v>1252</v>
+      </c>
+      <c r="F52">
+        <v>84</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52" t="s">
+        <v>30</v>
+      </c>
+      <c r="I52" t="s">
+        <v>200</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>278</v>
+      </c>
+      <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53">
+        <v>3000</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53" t="s">
+        <v>72</v>
+      </c>
+      <c r="I53" t="s">
+        <v>201</v>
+      </c>
+      <c r="J53">
+        <v>64</v>
+      </c>
+      <c r="K53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>180</v>
+      </c>
+      <c r="E54">
+        <v>180</v>
+      </c>
+      <c r="F54">
+        <v>51</v>
+      </c>
+      <c r="G54">
+        <v>6</v>
+      </c>
+      <c r="H54" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54" t="s">
+        <v>201</v>
+      </c>
+      <c r="J54">
+        <v>24</v>
+      </c>
+      <c r="K54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>130</v>
+      </c>
+      <c r="B55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1800</v>
+      </c>
+      <c r="E55">
+        <v>1965</v>
+      </c>
+      <c r="F55">
+        <v>750</v>
+      </c>
+      <c r="G55">
+        <v>42</v>
+      </c>
+      <c r="H55" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" t="s">
+        <v>200</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1800</v>
+      </c>
+      <c r="E56">
+        <v>1965</v>
+      </c>
+      <c r="F56">
+        <v>750</v>
+      </c>
+      <c r="G56">
+        <v>42</v>
+      </c>
+      <c r="H56" t="s">
+        <v>19</v>
+      </c>
+      <c r="I56" t="s">
+        <v>200</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>132</v>
+      </c>
+      <c r="B57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <v>30</v>
+      </c>
+      <c r="F57">
+        <v>570</v>
+      </c>
+      <c r="G57">
+        <v>4</v>
+      </c>
+      <c r="H57" t="s">
+        <v>23</v>
+      </c>
+      <c r="I57" t="s">
+        <v>200</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>267</v>
+      </c>
+      <c r="E58">
+        <v>173</v>
+      </c>
+      <c r="F58">
+        <v>144</v>
+      </c>
+      <c r="G58">
+        <v>7</v>
+      </c>
+      <c r="H58" t="s">
+        <v>135</v>
+      </c>
+      <c r="I58" t="s">
+        <v>201</v>
+      </c>
+      <c r="J58">
+        <v>963</v>
+      </c>
+      <c r="K58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>138</v>
+      </c>
+      <c r="B59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>214</v>
+      </c>
+      <c r="E59">
+        <v>1896</v>
+      </c>
+      <c r="F59">
+        <v>1024</v>
+      </c>
+      <c r="G59">
+        <v>39</v>
+      </c>
+      <c r="H59" t="s">
+        <v>139</v>
+      </c>
+      <c r="I59" t="s">
+        <v>200</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>50</v>
+      </c>
+      <c r="E60">
+        <v>50</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>10</v>
+      </c>
+      <c r="H60" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" t="s">
+        <v>200</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" t="s">
+        <v>142</v>
+      </c>
+      <c r="C61" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>104</v>
+      </c>
+      <c r="E61">
+        <v>208</v>
+      </c>
+      <c r="F61">
+        <v>2000</v>
+      </c>
+      <c r="G61">
+        <v>52</v>
+      </c>
+      <c r="H61" t="s">
+        <v>143</v>
+      </c>
+      <c r="I61" t="s">
+        <v>200</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>104</v>
+      </c>
+      <c r="E62">
+        <v>208</v>
+      </c>
+      <c r="F62">
+        <v>2000</v>
+      </c>
+      <c r="G62">
+        <v>52</v>
+      </c>
+      <c r="H62" t="s">
+        <v>143</v>
+      </c>
+      <c r="I62" t="s">
+        <v>200</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>145</v>
+      </c>
+      <c r="B63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>104</v>
+      </c>
+      <c r="E63">
+        <v>208</v>
+      </c>
+      <c r="F63">
+        <v>2000</v>
+      </c>
+      <c r="G63">
+        <v>52</v>
+      </c>
+      <c r="H63" t="s">
+        <v>143</v>
+      </c>
+      <c r="I63" t="s">
+        <v>200</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>146</v>
+      </c>
+      <c r="B64" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>537</v>
+      </c>
+      <c r="E64">
+        <v>537</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>11</v>
+      </c>
+      <c r="H64" t="s">
+        <v>3</v>
+      </c>
+      <c r="I64" t="s">
+        <v>200</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>105</v>
+      </c>
+      <c r="E65">
+        <v>105</v>
+      </c>
+      <c r="F65">
+        <v>144</v>
+      </c>
+      <c r="G65">
+        <v>7</v>
+      </c>
+      <c r="H65" t="s">
+        <v>30</v>
+      </c>
+      <c r="I65" t="s">
+        <v>200</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>148</v>
+      </c>
+      <c r="B66" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>180</v>
+      </c>
+      <c r="E66">
+        <v>180</v>
+      </c>
+      <c r="F66">
+        <v>144</v>
+      </c>
+      <c r="G66">
+        <v>2</v>
+      </c>
+      <c r="H66" t="s">
+        <v>3</v>
+      </c>
+      <c r="I66" t="s">
+        <v>200</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>152</v>
+      </c>
+      <c r="B67" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>151</v>
+      </c>
+      <c r="E67">
+        <v>152</v>
+      </c>
+      <c r="F67">
+        <v>30</v>
+      </c>
+      <c r="G67">
+        <v>4</v>
+      </c>
+      <c r="H67" t="s">
+        <v>21</v>
+      </c>
+      <c r="I67" t="s">
+        <v>201</v>
+      </c>
+      <c r="J67">
+        <v>6</v>
+      </c>
+      <c r="K67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>375</v>
+      </c>
+      <c r="E68">
+        <v>375</v>
+      </c>
+      <c r="F68">
+        <v>720</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68" t="s">
+        <v>3</v>
+      </c>
+      <c r="I68" t="s">
+        <v>200</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" t="s">
+        <v>155</v>
+      </c>
+      <c r="C69" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>20</v>
+      </c>
+      <c r="E69">
+        <v>50</v>
+      </c>
+      <c r="F69">
+        <v>2844</v>
+      </c>
+      <c r="G69">
+        <v>4</v>
+      </c>
+      <c r="H69" t="s">
+        <v>23</v>
+      </c>
+      <c r="I69" t="s">
+        <v>200</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>375</v>
+      </c>
+      <c r="E70">
+        <v>375</v>
+      </c>
+      <c r="F70">
+        <v>720</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70" t="s">
+        <v>3</v>
+      </c>
+      <c r="I70" t="s">
+        <v>200</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>157</v>
+      </c>
+      <c r="B71" t="s">
+        <v>157</v>
+      </c>
+      <c r="C71" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>268</v>
+      </c>
+      <c r="E71">
+        <v>293</v>
+      </c>
+      <c r="F71">
+        <v>896</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71" t="s">
+        <v>72</v>
+      </c>
+      <c r="I71" t="s">
+        <v>201</v>
+      </c>
+      <c r="J71">
+        <v>6</v>
+      </c>
+      <c r="K71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>158</v>
+      </c>
+      <c r="B72" t="s">
+        <v>158</v>
+      </c>
+      <c r="C72" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>200</v>
+      </c>
+      <c r="E72">
+        <v>180</v>
+      </c>
+      <c r="F72">
+        <v>1152</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72" t="s">
+        <v>72</v>
+      </c>
+      <c r="I72" t="s">
+        <v>201</v>
+      </c>
+      <c r="J72">
+        <v>7</v>
+      </c>
+      <c r="K72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>159</v>
+      </c>
+      <c r="B73" t="s">
+        <v>159</v>
+      </c>
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>300</v>
+      </c>
+      <c r="E73">
+        <v>600</v>
+      </c>
+      <c r="F73">
+        <v>1500</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+      <c r="H73" t="s">
+        <v>23</v>
+      </c>
+      <c r="I73" t="s">
+        <v>200</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>160</v>
+      </c>
+      <c r="B74" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>450</v>
+      </c>
+      <c r="E74">
+        <v>450</v>
+      </c>
+      <c r="F74">
+        <v>1500</v>
+      </c>
+      <c r="G74">
+        <v>6</v>
+      </c>
+      <c r="H74" t="s">
+        <v>23</v>
+      </c>
+      <c r="I74" t="s">
+        <v>200</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>161</v>
+      </c>
+      <c r="B75" t="s">
+        <v>161</v>
+      </c>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>450</v>
+      </c>
+      <c r="E75">
+        <v>450</v>
+      </c>
+      <c r="F75">
+        <v>1500</v>
+      </c>
+      <c r="G75">
+        <v>5</v>
+      </c>
+      <c r="H75" t="s">
+        <v>23</v>
+      </c>
+      <c r="I75" t="s">
+        <v>200</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>162</v>
+      </c>
+      <c r="B76" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>50</v>
+      </c>
+      <c r="E76">
+        <v>50</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>10</v>
+      </c>
+      <c r="H76" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" t="s">
+        <v>200</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="K76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>167</v>
+      </c>
+      <c r="B77" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>375</v>
+      </c>
+      <c r="E77">
+        <v>375</v>
+      </c>
+      <c r="F77">
+        <v>720</v>
+      </c>
+      <c r="G77">
+        <v>3</v>
+      </c>
+      <c r="H77" t="s">
+        <v>3</v>
+      </c>
+      <c r="I77" t="s">
+        <v>200</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>169</v>
+      </c>
+      <c r="B78" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>20</v>
+      </c>
+      <c r="E78">
+        <v>601</v>
+      </c>
+      <c r="F78">
+        <v>70</v>
+      </c>
+      <c r="G78">
+        <v>2</v>
+      </c>
+      <c r="H78" t="s">
+        <v>30</v>
+      </c>
+      <c r="I78" t="s">
+        <v>200</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="K78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>170</v>
+      </c>
+      <c r="B79" t="s">
+        <v>170</v>
+      </c>
+      <c r="C79" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>27</v>
+      </c>
+      <c r="E79">
+        <v>953</v>
+      </c>
+      <c r="F79">
+        <v>65</v>
+      </c>
+      <c r="G79">
+        <v>2</v>
+      </c>
+      <c r="H79" t="s">
+        <v>30</v>
+      </c>
+      <c r="I79" t="s">
+        <v>200</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="K79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>171</v>
+      </c>
+      <c r="B80" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" t="b">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>6599</v>
+      </c>
+      <c r="E80">
+        <v>2199</v>
+      </c>
+      <c r="F80">
+        <v>93</v>
+      </c>
+      <c r="G80">
+        <v>10</v>
+      </c>
+      <c r="H80" t="s">
+        <v>172</v>
+      </c>
+      <c r="I80" t="s">
+        <v>201</v>
+      </c>
+      <c r="J80">
+        <v>13</v>
+      </c>
+      <c r="K80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>173</v>
+      </c>
+      <c r="B81" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" t="b">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>12</v>
+      </c>
+      <c r="E81">
+        <v>15</v>
+      </c>
+      <c r="F81">
+        <v>2500</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+      <c r="H81" t="s">
+        <v>19</v>
+      </c>
+      <c r="I81" t="s">
+        <v>201</v>
+      </c>
+      <c r="J81">
+        <v>4</v>
+      </c>
+      <c r="K81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>174</v>
+      </c>
+      <c r="B82" t="s">
+        <v>174</v>
+      </c>
+      <c r="C82" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>1000</v>
+      </c>
+      <c r="E82">
+        <v>8236</v>
+      </c>
+      <c r="F82">
+        <v>1024</v>
+      </c>
+      <c r="G82">
+        <v>3</v>
+      </c>
+      <c r="H82" t="s">
+        <v>30</v>
+      </c>
+      <c r="I82" t="s">
+        <v>200</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" t="s">
+        <v>175</v>
+      </c>
+      <c r="C83" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>613</v>
+      </c>
+      <c r="E83">
+        <v>370</v>
+      </c>
+      <c r="F83">
+        <v>235</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83" t="s">
+        <v>23</v>
+      </c>
+      <c r="I83" t="s">
+        <v>200</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>182</v>
+      </c>
+      <c r="B84" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" t="b">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>100</v>
+      </c>
+      <c r="E84">
+        <v>100</v>
+      </c>
+      <c r="F84">
+        <v>275</v>
+      </c>
+      <c r="G84">
+        <v>4</v>
+      </c>
+      <c r="H84" t="s">
+        <v>30</v>
+      </c>
+      <c r="I84" t="s">
+        <v>200</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>183</v>
+      </c>
+      <c r="B85" t="s">
+        <v>183</v>
+      </c>
+      <c r="C85" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>23</v>
+      </c>
+      <c r="E85">
+        <v>1139</v>
+      </c>
+      <c r="F85">
+        <v>82</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="H85" t="s">
+        <v>19</v>
+      </c>
+      <c r="I85" t="s">
+        <v>200</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>187</v>
+      </c>
+      <c r="B86" t="s">
+        <v>187</v>
+      </c>
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>2238</v>
+      </c>
+      <c r="E86">
+        <v>2241</v>
+      </c>
+      <c r="F86">
+        <v>315</v>
+      </c>
+      <c r="G86">
+        <v>8</v>
+      </c>
+      <c r="H86" t="s">
+        <v>21</v>
+      </c>
+      <c r="I86" t="s">
+        <v>201</v>
+      </c>
+      <c r="J86">
+        <v>3</v>
+      </c>
+      <c r="K86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87" t="s">
+        <v>192</v>
+      </c>
+      <c r="C87" t="b">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1000</v>
+      </c>
+      <c r="E87">
+        <v>6164</v>
+      </c>
+      <c r="F87">
+        <v>152</v>
+      </c>
+      <c r="G87">
+        <v>2</v>
+      </c>
+      <c r="H87" t="s">
+        <v>30</v>
+      </c>
+      <c r="I87" t="s">
+        <v>200</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>193</v>
+      </c>
+      <c r="B88" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>57</v>
+      </c>
+      <c r="E88">
+        <v>54</v>
+      </c>
+      <c r="F88">
+        <v>234</v>
+      </c>
+      <c r="G88">
+        <v>2</v>
+      </c>
+      <c r="H88" t="s">
+        <v>23</v>
+      </c>
+      <c r="I88" t="s">
+        <v>200</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="K88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified prepare reports ammended last changes
</commit_message>
<xml_diff>
--- a/Datasets_metadata.xlsx
+++ b/Datasets_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alo/Documents/master-thesis/Master-Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0446FCAC-8CE8-5746-8E48-7AE987CA0125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574ADC55-5FFB-7A4B-8D22-4A1EBDA7C8D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1741" uniqueCount="228">
   <si>
     <t>AbnormalHeartbeat</t>
   </si>
@@ -704,19 +704,22 @@
     <t>10% failed</t>
   </si>
   <si>
-    <t>RuntimeError: No shapelets were extracted in fit that exceeded the minimum information gain threshold. Please retry with other data and/or parameter settings.</t>
-  </si>
-  <si>
     <t>change min window</t>
   </si>
   <si>
     <t>100% failed, use defaule split</t>
   </si>
   <si>
-    <t>Liblinear failed to converge, increase the number of iterations.</t>
-  </si>
-  <si>
-    <t>large  number of dimensions, for weasel Liblinear failed to converge, increase the number of iterations.</t>
+    <t>it runs as no cv for weasel and I should run 100 %</t>
+  </si>
+  <si>
+    <t>run 100 for weasel</t>
+  </si>
+  <si>
+    <t>default_split</t>
+  </si>
+  <si>
+    <t>run next for weasel, after adding more the chunks</t>
   </si>
 </sst>
 </file>
@@ -831,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -852,6 +855,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1474,6 +1480,24 @@
         <filter val="TRUE"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="AUDIO"/>
+        <filter val="DEVICE"/>
+        <filter val="ECG"/>
+        <filter val="EEG"/>
+        <filter val="EOG"/>
+        <filter val="EPG"/>
+        <filter val="HAR"/>
+        <filter val="HEMODYNAMICS"/>
+        <filter val="MISC"/>
+        <filter val="OTHER"/>
+        <filter val="SENSOR"/>
+        <filter val="SOUND"/>
+        <filter val="SPECTRO"/>
+        <filter val="SPEECH"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E179">
     <sortCondition ref="A1:A179"/>
@@ -1854,7 +1878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N179"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -7689,8 +7713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="L70" sqref="L70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7803,7 +7827,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -7831,7 +7855,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -7859,7 +7883,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -7887,7 +7911,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -7915,7 +7939,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -7943,7 +7967,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -8140,10 +8164,12 @@
         <v>1</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
       <c r="K16" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L16" s="4"/>
     </row>
@@ -8192,24 +8218,28 @@
       <c r="E18" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
       <c r="G18" s="4">
         <v>1</v>
       </c>
       <c r="H18" s="4">
         <v>1</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4">
+        <v>1</v>
+      </c>
       <c r="J18" s="4">
         <v>1</v>
       </c>
       <c r="K18" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
@@ -8261,7 +8291,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
@@ -8289,7 +8319,7 @@
       </c>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>27</v>
       </c>
@@ -8341,11 +8371,15 @@
       <c r="H23" s="4">
         <v>1</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="I23" s="4">
+        <v>1</v>
+      </c>
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
       <c r="K23" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L23" s="4"/>
     </row>
@@ -8373,7 +8407,7 @@
       </c>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>32</v>
       </c>
@@ -8401,7 +8435,7 @@
       </c>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
@@ -8429,7 +8463,7 @@
       </c>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>34</v>
       </c>
@@ -8464,10 +8498,10 @@
         <v>3</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
@@ -8559,13 +8593,15 @@
       <c r="H30" s="4">
         <v>1</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="I30" s="4">
+        <v>1</v>
+      </c>
       <c r="J30" s="4">
         <v>1</v>
       </c>
       <c r="K30" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L30" s="4"/>
     </row>
@@ -8681,7 +8717,7 @@
       </c>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
@@ -8709,7 +8745,7 @@
       </c>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
@@ -8737,7 +8773,7 @@
       </c>
       <c r="L36" s="4"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>45</v>
       </c>
@@ -8765,7 +8801,7 @@
       </c>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>46</v>
       </c>
@@ -8793,7 +8829,7 @@
       </c>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>47</v>
       </c>
@@ -8821,7 +8857,7 @@
       </c>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>48</v>
       </c>
@@ -8849,7 +8885,7 @@
       </c>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>49</v>
       </c>
@@ -8877,7 +8913,7 @@
       </c>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>50</v>
       </c>
@@ -8929,11 +8965,15 @@
       <c r="H43" s="4">
         <v>1</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="I43" s="4">
+        <v>1</v>
+      </c>
+      <c r="J43" s="4">
+        <v>1</v>
+      </c>
       <c r="K43" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L43" s="4"/>
     </row>
@@ -8966,10 +9006,12 @@
       <c r="I44" s="4">
         <v>1</v>
       </c>
-      <c r="J44" s="4"/>
+      <c r="J44" s="4">
+        <v>1</v>
+      </c>
       <c r="K44" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L44" s="4"/>
     </row>
@@ -8990,7 +9032,9 @@
       <c r="E45" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="F45" s="4"/>
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
       <c r="G45" s="4">
         <v>1</v>
       </c>
@@ -9000,43 +9044,47 @@
       <c r="I45" s="4">
         <v>1</v>
       </c>
-      <c r="J45" s="4"/>
+      <c r="J45" s="4">
+        <v>1</v>
+      </c>
       <c r="K45" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="5" t="b">
-        <f>IF(Table13[[#This Row],[dataset]]=Table13[[#This Row],[uea_ucr]],TRUE,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" s="5" t="s">
+      <c r="C46" s="7" t="b">
+        <f>IF(Table13[[#This Row],[dataset]]=Table13[[#This Row],[uea_ucr]],TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4">
-        <v>0</v>
-      </c>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4">
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
+        <v>1</v>
+      </c>
+      <c r="I46" s="6">
+        <v>0</v>
+      </c>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L46" s="4" t="s">
-        <v>225</v>
+        <v>1</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -9090,10 +9138,12 @@
       <c r="I48" s="4">
         <v>1</v>
       </c>
-      <c r="J48" s="4"/>
+      <c r="J48" s="4">
+        <v>1</v>
+      </c>
       <c r="K48" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L48" s="4"/>
     </row>
@@ -9191,7 +9241,7 @@
       </c>
       <c r="L51" s="4"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>60</v>
       </c>
@@ -9276,7 +9326,7 @@
         <v>4</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -9388,14 +9438,16 @@
       <c r="E58" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F58" s="4"/>
+      <c r="F58" s="4">
+        <v>1</v>
+      </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58" s="4"/>
     </row>
@@ -9491,7 +9543,7 @@
       </c>
       <c r="L61" s="4"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>73</v>
       </c>
@@ -9520,7 +9572,7 @@
       <c r="L62" s="4"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B63" s="5" t="s">
@@ -9550,10 +9602,10 @@
         <v>0</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>75</v>
       </c>
@@ -9581,7 +9633,7 @@
       </c>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>76</v>
       </c>
@@ -9609,7 +9661,7 @@
       </c>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>77</v>
       </c>
@@ -9665,7 +9717,7 @@
       </c>
       <c r="L67" s="4"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>79</v>
       </c>
@@ -9720,10 +9772,12 @@
       <c r="I69" s="4">
         <v>1</v>
       </c>
-      <c r="J69" s="4"/>
+      <c r="J69" s="4">
+        <v>1</v>
+      </c>
       <c r="K69" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L69" s="4"/>
     </row>
@@ -9754,10 +9808,12 @@
       <c r="I70" s="4">
         <v>1</v>
       </c>
-      <c r="J70" s="4"/>
+      <c r="J70" s="4">
+        <v>1</v>
+      </c>
       <c r="K70" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L70" s="4" t="s">
         <v>220</v>
@@ -9790,10 +9846,12 @@
       <c r="I71" s="4">
         <v>1</v>
       </c>
-      <c r="J71" s="4"/>
+      <c r="J71" s="4">
+        <v>1</v>
+      </c>
       <c r="K71" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L71" s="4"/>
     </row>
@@ -9814,7 +9872,9 @@
       <c r="E72" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="F72" s="4"/>
+      <c r="F72" s="4">
+        <v>1</v>
+      </c>
       <c r="G72" s="4">
         <v>1</v>
       </c>
@@ -9824,10 +9884,12 @@
       <c r="I72" s="4">
         <v>1</v>
       </c>
-      <c r="J72" s="4"/>
+      <c r="J72" s="4">
+        <v>1</v>
+      </c>
       <c r="K72" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L72" s="4"/>
     </row>
@@ -9889,7 +9951,7 @@
       </c>
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>86</v>
       </c>
@@ -9917,7 +9979,7 @@
       </c>
       <c r="L75" s="4"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>87</v>
       </c>
@@ -9945,7 +10007,7 @@
       </c>
       <c r="L76" s="4"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>88</v>
       </c>
@@ -9973,7 +10035,7 @@
       </c>
       <c r="L77" s="4"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>89</v>
       </c>
@@ -10001,7 +10063,7 @@
       </c>
       <c r="L78" s="4"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>90</v>
       </c>
@@ -10029,7 +10091,7 @@
       </c>
       <c r="L79" s="4"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>91</v>
       </c>
@@ -10057,7 +10119,7 @@
       </c>
       <c r="L80" s="4"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>92</v>
       </c>
@@ -10085,7 +10147,7 @@
       </c>
       <c r="L81" s="4"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>93</v>
       </c>
@@ -10113,7 +10175,7 @@
       </c>
       <c r="L82" s="4"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>94</v>
       </c>
@@ -10207,7 +10269,7 @@
       </c>
       <c r="L85" s="4"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>97</v>
       </c>
@@ -10263,7 +10325,7 @@
       </c>
       <c r="L87" s="4"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>99</v>
       </c>
@@ -10292,7 +10354,7 @@
       <c r="L88" s="4"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="15" t="s">
         <v>100</v>
       </c>
       <c r="B89" s="5" t="s">
@@ -10320,10 +10382,10 @@
         <v>0</v>
       </c>
       <c r="L89" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>101</v>
       </c>
@@ -10387,7 +10449,7 @@
       </c>
       <c r="L91" s="4"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>103</v>
       </c>
@@ -10600,13 +10662,15 @@
       <c r="I98" s="4">
         <v>1</v>
       </c>
-      <c r="J98" s="4"/>
+      <c r="J98" s="4">
+        <v>1</v>
+      </c>
       <c r="K98" s="4">
         <f t="shared" ref="K98:K129" si="3">SUM(F98:J98)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
@@ -10640,7 +10704,7 @@
         <v>1</v>
       </c>
       <c r="L99" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.2">
@@ -10736,10 +10800,12 @@
       <c r="I102" s="4">
         <v>1</v>
       </c>
-      <c r="J102" s="4"/>
+      <c r="J102" s="4">
+        <v>1</v>
+      </c>
       <c r="K102" s="4">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L102" s="4" t="s">
         <v>221</v>
@@ -10772,10 +10838,12 @@
       <c r="I103" s="4">
         <v>1</v>
       </c>
-      <c r="J103" s="4"/>
+      <c r="J103" s="4">
+        <v>1</v>
+      </c>
       <c r="K103" s="4">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L103" s="4"/>
     </row>
@@ -10807,7 +10875,7 @@
       </c>
       <c r="L104" s="4"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>116</v>
       </c>
@@ -10871,7 +10939,7 @@
       </c>
       <c r="L106" s="4"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>118</v>
       </c>
@@ -10899,7 +10967,7 @@
       </c>
       <c r="L107" s="4"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>119</v>
       </c>
@@ -10932,10 +11000,10 @@
         <v>2</v>
       </c>
       <c r="L108" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>121</v>
       </c>
@@ -10963,7 +11031,7 @@
       </c>
       <c r="L109" s="4"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>122</v>
       </c>
@@ -10991,7 +11059,7 @@
       </c>
       <c r="L110" s="4"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>123</v>
       </c>
@@ -11019,7 +11087,7 @@
       </c>
       <c r="L111" s="4"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>124</v>
       </c>
@@ -11047,7 +11115,7 @@
       </c>
       <c r="L112" s="4"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>125</v>
       </c>
@@ -11128,15 +11196,17 @@
       <c r="I115" s="4">
         <v>1</v>
       </c>
-      <c r="J115" s="4"/>
+      <c r="J115" s="4">
+        <v>1</v>
+      </c>
       <c r="K115" s="4">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L115" s="4"/>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="15" t="s">
         <v>128</v>
       </c>
       <c r="B116" s="5" t="s">
@@ -11156,15 +11226,15 @@
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J116" s="4"/>
       <c r="K116" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L116" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
@@ -11195,7 +11265,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L117" s="4"/>
+      <c r="L117" s="6" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
@@ -11309,7 +11381,7 @@
       </c>
       <c r="L120" s="4"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>133</v>
       </c>
@@ -11338,7 +11410,7 @@
       <c r="L121" s="4"/>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="15" t="s">
         <v>134</v>
       </c>
       <c r="B122" s="5" t="s">
@@ -11366,10 +11438,10 @@
         <v>0</v>
       </c>
       <c r="L122" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>136</v>
       </c>
@@ -11397,7 +11469,7 @@
       </c>
       <c r="L123" s="4"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>137</v>
       </c>
@@ -11512,10 +11584,12 @@
       <c r="I127" s="4">
         <v>1</v>
       </c>
-      <c r="J127" s="4"/>
+      <c r="J127" s="4">
+        <v>1</v>
+      </c>
       <c r="K127" s="4">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L127" s="4"/>
     </row>
@@ -11678,10 +11752,12 @@
       <c r="I132" s="4">
         <v>1</v>
       </c>
-      <c r="J132" s="4"/>
+      <c r="J132" s="4">
+        <v>1</v>
+      </c>
       <c r="K132" s="4">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L132" s="4"/>
     </row>
@@ -11723,7 +11799,7 @@
       </c>
       <c r="L133" s="4"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>149</v>
       </c>
@@ -11751,7 +11827,7 @@
       </c>
       <c r="L134" s="4"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>150</v>
       </c>
@@ -11779,7 +11855,7 @@
       </c>
       <c r="L135" s="4"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>151</v>
       </c>
@@ -12162,14 +12238,16 @@
       <c r="I147" s="4">
         <v>1</v>
       </c>
-      <c r="J147" s="4"/>
+      <c r="J147" s="4">
+        <v>1</v>
+      </c>
       <c r="K147" s="4">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L147" s="4"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>163</v>
       </c>
@@ -12197,7 +12275,7 @@
       </c>
       <c r="L148" s="4"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>164</v>
       </c>
@@ -12285,7 +12363,7 @@
       </c>
       <c r="L151" s="4"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>168</v>
       </c>
@@ -12342,10 +12420,12 @@
       <c r="I153" s="4">
         <v>1</v>
       </c>
-      <c r="J153" s="4"/>
+      <c r="J153" s="4">
+        <v>1</v>
+      </c>
       <c r="K153" s="4">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L153" s="4"/>
     </row>
@@ -12378,45 +12458,49 @@
       <c r="I154" s="4">
         <v>1</v>
       </c>
-      <c r="J154" s="4"/>
+      <c r="J154" s="4">
+        <v>1</v>
+      </c>
       <c r="K154" s="4">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L154" s="4"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A155" s="4" t="s">
+    <row r="155" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="B155" s="5" t="s">
+      <c r="B155" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C155" s="5" t="b">
-        <f>IF(Table13[[#This Row],[dataset]]=Table13[[#This Row],[uea_ucr]],TRUE,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="D155" s="4" t="s">
+      <c r="C155" s="7" t="b">
+        <f>IF(Table13[[#This Row],[dataset]]=Table13[[#This Row],[uea_ucr]],TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D155" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E155" s="5" t="s">
+      <c r="E155" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="F155" s="4"/>
-      <c r="G155" s="4">
-        <v>0</v>
-      </c>
-      <c r="H155" s="4">
-        <v>0</v>
-      </c>
-      <c r="I155" s="4"/>
-      <c r="J155" s="4"/>
-      <c r="K155" s="4">
+      <c r="F155" s="6"/>
+      <c r="G155" s="6">
+        <v>0</v>
+      </c>
+      <c r="H155" s="6">
+        <v>0</v>
+      </c>
+      <c r="I155" s="6"/>
+      <c r="J155" s="6">
+        <v>0</v>
+      </c>
+      <c r="K155" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L155" s="4" t="s">
-        <v>222</v>
+      <c r="L155" s="6" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
@@ -12523,7 +12607,7 @@
       </c>
       <c r="L158" s="4"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>176</v>
       </c>
@@ -12551,7 +12635,7 @@
       </c>
       <c r="L159" s="4"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>177</v>
       </c>
@@ -12579,7 +12663,7 @@
       </c>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>178</v>
       </c>
@@ -12631,7 +12715,7 @@
       </c>
       <c r="L162" s="4"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>180</v>
       </c>
@@ -12659,7 +12743,7 @@
       </c>
       <c r="L163" s="4"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>181</v>
       </c>
@@ -12714,10 +12798,12 @@
       <c r="I165" s="4">
         <v>1</v>
       </c>
-      <c r="J165" s="4"/>
+      <c r="J165" s="4">
+        <v>1</v>
+      </c>
       <c r="K165" s="4">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L165" s="4"/>
     </row>
@@ -12755,7 +12841,7 @@
       </c>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>184</v>
       </c>
@@ -12783,7 +12869,7 @@
       </c>
       <c r="L167" s="4"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>185</v>
       </c>
@@ -12863,7 +12949,7 @@
       </c>
       <c r="L170" s="4"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>188</v>
       </c>
@@ -12891,7 +12977,7 @@
       </c>
       <c r="L171" s="4"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>189</v>
       </c>
@@ -12919,7 +13005,7 @@
       </c>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>190</v>
       </c>
@@ -12947,7 +13033,7 @@
       </c>
       <c r="L173" s="4"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>191</v>
       </c>
@@ -13002,10 +13088,12 @@
       <c r="I175" s="4">
         <v>1</v>
       </c>
-      <c r="J175" s="4"/>
+      <c r="J175" s="4">
+        <v>1</v>
+      </c>
       <c r="K175" s="4">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L175" s="4"/>
     </row>
@@ -13045,7 +13133,7 @@
       </c>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>194</v>
       </c>
@@ -13073,7 +13161,7 @@
       </c>
       <c r="L177" s="4"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>195</v>
       </c>
@@ -13101,7 +13189,7 @@
       </c>
       <c r="L178" s="4"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>196</v>
       </c>
@@ -13129,7 +13217,7 @@
       </c>
       <c r="L179" s="4"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>197</v>
       </c>
@@ -13186,8 +13274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13521,7 +13609,7 @@
       <c r="P9" s="12"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="14" t="s">
         <v>53</v>
       </c>
       <c r="B10" t="s">
@@ -13732,7 +13820,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="14" t="s">
         <v>83</v>
       </c>
       <c r="B16" t="s">
@@ -13767,7 +13855,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="14" t="s">
         <v>67</v>
       </c>
       <c r="B17" t="s">
@@ -13802,7 +13890,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
@@ -14081,38 +14169,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="16">
         <v>60</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="16">
         <v>40</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="16">
         <v>270</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="16">
         <v>5</v>
       </c>
-      <c r="H26" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="H26" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="16">
         <v>1345</v>
       </c>
-      <c r="K26" t="b">
+      <c r="K26" s="16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14991,38 +15079,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="52" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C52" t="b">
-        <v>1</v>
-      </c>
-      <c r="D52">
+      <c r="C52" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" s="16">
         <v>204</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="16">
         <v>205</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="16">
         <v>405</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="16">
         <v>2</v>
       </c>
-      <c r="H52" t="s">
-        <v>1</v>
-      </c>
-      <c r="I52" t="s">
+      <c r="H52" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I52" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="16">
         <v>61</v>
       </c>
-      <c r="K52" t="b">
+      <c r="K52" s="16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -15131,38 +15219,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="56" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="C56" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56">
+      <c r="C56" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="16">
         <v>267</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="16">
         <v>173</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="16">
         <v>144</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="16">
         <v>7</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="16">
         <v>963</v>
       </c>
-      <c r="K56" t="b">
+      <c r="K56" s="16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -15236,38 +15324,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="59" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C59" t="b">
-        <v>1</v>
-      </c>
-      <c r="D59">
+      <c r="C59" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" s="16">
         <v>278</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="16">
         <v>100</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="16">
         <v>3000</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="16">
         <v>2</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="16">
         <v>64</v>
       </c>
-      <c r="K59" t="b">
+      <c r="K59" s="16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -16111,38 +16199,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="84" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C84" t="b">
-        <v>1</v>
-      </c>
-      <c r="D84">
+      <c r="C84" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D84" s="16">
         <v>5890</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="16">
         <v>3524</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="16">
         <v>62</v>
       </c>
-      <c r="G84">
+      <c r="G84" s="16">
         <v>2</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I84" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="J84">
+      <c r="J84" s="16">
         <v>144</v>
       </c>
-      <c r="K84" t="b">
+      <c r="K84" s="16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -16251,38 +16339,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="88" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C88" t="b">
-        <v>1</v>
-      </c>
-      <c r="D88">
+      <c r="C88" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88" s="16">
         <v>30000</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="16">
         <v>20000</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="16">
         <v>30</v>
       </c>
-      <c r="G88">
+      <c r="G88" s="16">
         <v>10</v>
       </c>
-      <c r="H88" t="s">
-        <v>1</v>
-      </c>
-      <c r="I88" t="s">
+      <c r="H88" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I88" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="J88">
-        <v>200</v>
-      </c>
-      <c r="K88" t="b">
+      <c r="J88" s="16">
+        <v>200</v>
+      </c>
+      <c r="K88" s="16" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>